<commit_message>
MINOR TWEAK: I forgot to turn loudness into a percentage. Mention to John.
</commit_message>
<xml_diff>
--- a/Joshua_Santiago-Francia_Assesment.xlsx
+++ b/Joshua_Santiago-Francia_Assesment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iadt-my.sharepoint.com/personal/n00151146_iadt_ie/Documents/Y2/Creative Coding/John/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1751" documentId="11_99C22FBFB68F2B0FADA4AE43E2F8B2F38ABC2276" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0D13D92-9DE0-40C6-9C23-41EA342670B4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{EA0AB376-8246-459B-9C03-73819DF4ED03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Finn Nankivel" sheetId="32" r:id="rId1"/>
@@ -32,8 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="76">
   <si>
     <t>Creative Computing - First Year Prototyping Assesment Sheet</t>
   </si>
@@ -262,17 +260,20 @@
     <t>∑</t>
   </si>
   <si>
-    <t xml:space="preserve">∑ </t>
-  </si>
-  <si>
-    <t>During this project I learned a few things in Javascript such using push and pop + more about the co-ordinate system in p5. This was helpful for drawing ticks and labels, as well as legends for charts with multiple  yValues. I've also been out of secondary school for a while so things like learning how to create graphs with math was 'new' to me, as I previously would've just hardcoded their dimensions. During this assignment I also got refamiliarised with using the DOM and using it in tandem with event listeners to dynamically update scripts. For example changing the bar colours, widths, etc without having to submit a form. I also learned more advanced functions for grabbing data from arrays through messing with the cleanData() function in my sketch. Because I had so many different columns in my chart, I had to find a way to handle and process multiple data sets efficiently. This led me to explore array methods like map(), reduce() and Object.entries() which made manipulating the data more streamlined. Additionally, I gained a better understanding of how to structure classes in JavaScript, particularly when designing reusable components for charts. Unfortunately I had trouble getting my scripts to work within if functions when I tried to combine them into one 'chart' class, which lead me to abandon the endeavour before submission. I also would have loved to find a way to update the chart's background with javascript as my experimentation with that also didn't pan out well. If I had more time I believe I could've refactored a lot of my code and removed excess reuse (especially within the HTML document and the chart axis/label functions) of code to make it look more streamlined and less messy to look at.</t>
+    <t>The chart is mostly customisable except for the chart's canvas size</t>
+  </si>
+  <si>
+    <t>During this project I learned a few things in Javascript such using push and pop + more about the co-ordinate system in p5. This was helpful for drawing ticks and labels, as well as legends for charts with multiple  yValues. I've also been out of secondary school for a while so things like learning how to create graphs with math was 'new' to me, as I previously would've just hardcoded their dimensions. During this assignment I also got refamiliarised with using the DOM and using it in tandem with event listeners to dynamically update scripts. For example changing the bar colours, widths, etc without having to submit a form which is what I initially had but I changed it once I found the correct event listener to get input values. I also learned more advanced functions for grabbing data from arrays through messing with the cleanData() function in my sketch. Because I had so many different columns in my chart, I had to find a way to handle and process multiple data sets efficiently. This led me to explore array methods like map(), reduce() and Object.entries() which made manipulating the data more streamlined. Additionally, I gained a better understanding of how to structure classes in JavaScript, particularly when designing reusable components for charts. Unfortunately I had trouble getting my scripts to work within if/else functions when I tried to combine them into one master 'chart' class, which lead me to abandon the endeavour before submission. I also would have loved to find a way to update the chart's background with javascript as my experimentation with that also didn't pan out well. If I had more time I believe I could've refactored a lot of my code and removed excess reuse (especially within the HTML document and the chart axis/label functions) of code to make it look more streamlined and less messy to look at.</t>
+  </si>
+  <si>
+    <t>I don't think so.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,12 +561,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -601,45 +641,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1089,13 +1090,13 @@
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="8" width="15.140625" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1106,27 +1107,27 @@
         <v>44867</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="27" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="36"/>
-    </row>
-    <row r="4" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:8" ht="27" customHeight="1">
       <c r="A4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1153,7 +1154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1162,19 +1163,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
@@ -1194,7 +1195,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1206,10 +1207,10 @@
       <c r="G13" s="12"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1241,10 +1242,10 @@
       <c r="G16" s="12"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1276,10 +1277,10 @@
       <c r="G19" s="12"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -1299,7 +1300,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -1311,10 +1312,10 @@
       <c r="G22" s="12"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="G23" s="13"/>
     </row>
-    <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
@@ -1334,7 +1335,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -1346,46 +1347,46 @@
       <c r="G25" s="12"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
+    <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
-    </row>
-    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="20"/>
-    </row>
-    <row r="30" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
-    </row>
-    <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
+    </row>
+    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+    </row>
+    <row r="30" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="33"/>
+    </row>
+    <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>24</v>
       </c>
@@ -1394,210 +1395,210 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+    <row r="33" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A33" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21" t="s">
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="23"/>
-    </row>
-    <row r="34" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="36"/>
+    </row>
+    <row r="34" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A34" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21" t="s">
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="23"/>
-    </row>
-    <row r="35" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="36"/>
+    </row>
+    <row r="35" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A35" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21" t="s">
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="23"/>
-    </row>
-    <row r="36" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="36"/>
+    </row>
+    <row r="36" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A36" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21" t="s">
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="23"/>
-    </row>
-    <row r="37" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="36"/>
+    </row>
+    <row r="37" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A37" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21" t="s">
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="23"/>
-    </row>
-    <row r="38" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="36"/>
+    </row>
+    <row r="38" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A38" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21" t="s">
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="23"/>
-    </row>
-    <row r="39" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="36"/>
+    </row>
+    <row r="39" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A39" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21" t="s">
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="23"/>
-    </row>
-    <row r="40" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="36"/>
+    </row>
+    <row r="40" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A40" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21" t="s">
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="23"/>
-    </row>
-    <row r="41" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="36"/>
+    </row>
+    <row r="41" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A41" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21" t="s">
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="23"/>
-    </row>
-    <row r="42" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36"/>
+    </row>
+    <row r="42" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A42" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="21" t="s">
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="23"/>
-    </row>
-    <row r="43" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="36"/>
+    </row>
+    <row r="43" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A43" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="21" t="s">
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="23"/>
-    </row>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="36"/>
+    </row>
+    <row r="44" spans="1:8" ht="12.75" customHeight="1"/>
+    <row r="45" spans="1:8" ht="18" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
+    <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A46" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="26"/>
-    </row>
-    <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="29"/>
-    </row>
-    <row r="48" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="32"/>
-    </row>
-    <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="39"/>
+    </row>
+    <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A47" s="40"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="42"/>
+    </row>
+    <row r="48" spans="1:8" ht="69.75" customHeight="1">
+      <c r="A48" s="43"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="45"/>
+    </row>
+    <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="10" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="9" t="s">
         <v>41</v>
       </c>
@@ -1623,7 +1624,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1633,13 +1634,13 @@
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" s="10" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="9" t="s">
         <v>41</v>
       </c>
@@ -1665,7 +1666,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="7" t="s">
         <v>18</v>
       </c>
@@ -1677,8 +1678,8 @@
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
     </row>
-    <row r="58" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>50</v>
       </c>
@@ -1686,8 +1687,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -1698,24 +1699,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="A28:H30"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="E39:H39"/>
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="E43:H43"/>
     <mergeCell ref="A46:H48"/>
@@ -1725,6 +1708,24 @@
     <mergeCell ref="E41:H41"/>
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="E42:H42"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="A28:H30"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E33:H33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -1742,17 +1743,17 @@
   </sheetPr>
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="8" width="15.140625" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -1763,27 +1764,27 @@
         <v>45714</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="27" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H3" s="36"/>
-    </row>
-    <row r="4" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:8" ht="27" customHeight="1">
       <c r="A4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1794,16 +1795,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="19" t="s">
         <v>72</v>
       </c>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>58</v>
       </c>
@@ -1812,7 +1813,7 @@
       </c>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1821,19 +1822,19 @@
       </c>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="E10" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>59</v>
       </c>
@@ -1853,7 +1854,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1863,10 +1864,10 @@
       <c r="G13" s="12"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>60</v>
       </c>
@@ -1886,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1896,10 +1897,10 @@
       <c r="G16" s="12"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>61</v>
       </c>
@@ -1919,7 +1920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1929,10 +1930,10 @@
       <c r="G19" s="12"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>67</v>
       </c>
@@ -1952,7 +1953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -1962,10 +1963,10 @@
       <c r="G22" s="12"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="G23" s="13"/>
     </row>
-    <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -1995,44 +1996,44 @@
       <c r="G25" s="12"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
-    </row>
-    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="20"/>
-    </row>
-    <row r="30" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="44"/>
-    </row>
-    <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
+    </row>
+    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+    </row>
+    <row r="30" spans="1:8" ht="63.75" customHeight="1">
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="33"/>
+    </row>
+    <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>24</v>
       </c>
@@ -2044,13 +2045,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+    <row r="33" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A33" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="16" t="s">
         <v>72</v>
       </c>
@@ -2058,13 +2059,13 @@
       <c r="G33" s="17"/>
       <c r="H33" s="18"/>
     </row>
-    <row r="34" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+    <row r="34" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A34" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="16" t="s">
         <v>72</v>
       </c>
@@ -2072,13 +2073,13 @@
       <c r="G34" s="17"/>
       <c r="H34" s="18"/>
     </row>
-    <row r="35" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+    <row r="35" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A35" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="16" t="s">
         <v>72</v>
       </c>
@@ -2086,13 +2087,13 @@
       <c r="G35" s="17"/>
       <c r="H35" s="18"/>
     </row>
-    <row r="36" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+    <row r="36" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A36" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="16" t="s">
         <v>72</v>
       </c>
@@ -2100,13 +2101,13 @@
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A37" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="16" t="s">
         <v>73</v>
       </c>
@@ -2114,13 +2115,13 @@
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+    <row r="38" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A38" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
       <c r="E38" s="16" t="s">
         <v>72</v>
       </c>
@@ -2128,13 +2129,13 @@
       <c r="G38" s="17"/>
       <c r="H38" s="18"/>
     </row>
-    <row r="39" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+    <row r="39" spans="1:8" s="15" customFormat="1" ht="35.1" customHeight="1">
+      <c r="A39" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="30"/>
       <c r="E39" s="16" t="s">
         <v>72</v>
       </c>
@@ -2142,56 +2143,56 @@
       <c r="G39" s="17"/>
       <c r="H39" s="18"/>
     </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="12.75" customHeight="1"/>
+    <row r="41" spans="1:8" ht="18" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+    <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A42" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="26"/>
-    </row>
-    <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="29"/>
-    </row>
-    <row r="44" spans="1:8" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="32"/>
-    </row>
-    <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="39"/>
+    </row>
+    <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="40"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="42"/>
+    </row>
+    <row r="44" spans="1:8" ht="69.75" customHeight="1">
+      <c r="A44" s="43"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="45"/>
+    </row>
+    <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:8" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" s="10" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="9" t="s">
         <v>41</v>
       </c>
@@ -2217,7 +2218,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -2229,13 +2230,13 @@
       </c>
       <c r="H49" s="7"/>
     </row>
-    <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="10" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="9" t="s">
         <v>41</v>
       </c>
@@ -2261,7 +2262,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -2271,14 +2272,14 @@
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="20.100000000000001" customHeight="1"/>
+    <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -2289,6 +2290,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="A28:H30"/>
+    <mergeCell ref="A33:D33"/>
     <mergeCell ref="A42:H44"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:D38"/>
@@ -2296,11 +2302,6 @@
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A36:D36"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="A28:H30"/>
-    <mergeCell ref="A33:D33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2312,23 +2313,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="dd339124-9524-4215-82c6-192425842893" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A19EDCE8CA784A4A8A6FFD66014235D1" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf735423e234db6ad1047a13e317d06d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dd339124-9524-4215-82c6-192425842893" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a47e241ce09424dc868ea6ee433f1dfe" ns2:_="">
     <xsd:import namespace="dd339124-9524-4215-82c6-192425842893"/>
@@ -2478,25 +2462,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFD4CE3E-DBC6-43C0-9822-7F1BC5386216}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dd339124-9524-4215-82c6-192425842893"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D5DADAB-3274-48BB-AB3E-7C5AD55E7D1A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="dd339124-9524-4215-82c6-192425842893" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50ABFD72-4958-4372-A412-8CB071E195F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2512,4 +2495,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D5DADAB-3274-48BB-AB3E-7C5AD55E7D1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFD4CE3E-DBC6-43C0-9822-7F1BC5386216}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dd339124-9524-4215-82c6-192425842893"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>